<commit_message>
Second round of coding. Getting into some shape now.
</commit_message>
<xml_diff>
--- a/data_architect_misc/kf_generator/Key-Figures_Files_Req_Specification.xlsx
+++ b/data_architect_misc/kf_generator/Key-Figures_Files_Req_Specification.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Output-Files_Especification" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Output-Files_Especification'!$B$25:$I$47</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Output-Files_Especification'!$A$25:$I$47</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="75">
   <si>
     <t>File Type</t>
   </si>
@@ -898,12 +898,15 @@
       </rPr>
       <t xml:space="preserve"> = Current Year</t>
     </r>
+  </si>
+  <si>
+    <t>1.5millions rows per file</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1685,6 +1688,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="13" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1748,20 +1754,17 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1800,7 +1803,7 @@
         <xdr:cNvPr id="2" name="Imagen 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{921CB379-B0A3-4CB7-AAE9-974F0EDBB619}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{921CB379-B0A3-4CB7-AAE9-974F0EDBB619}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2096,14 +2099,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4:H8"/>
+    <sheetView tabSelected="1" topLeftCell="C44" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G46" sqref="G46:G47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="88.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="88.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="22" style="1" customWidth="1"/>
@@ -2117,71 +2120,74 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="23.25" x14ac:dyDescent="0.2">
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="50" t="s">
         <v>62</v>
       </c>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
     </row>
     <row r="3" spans="2:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="48" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="54" t="s">
+      <c r="C4" s="55" t="s">
         <v>63</v>
       </c>
-      <c r="D4" s="55"/>
-      <c r="E4" s="55"/>
-      <c r="F4" s="56"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="56"/>
+      <c r="F4" s="57"/>
     </row>
     <row r="5" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="48" t="s">
         <v>51</v>
       </c>
-      <c r="C5" s="57" t="s">
+      <c r="C5" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="D5" s="58"/>
-      <c r="E5" s="58"/>
-      <c r="F5" s="59"/>
+      <c r="D5" s="59"/>
+      <c r="E5" s="59"/>
+      <c r="F5" s="60"/>
     </row>
     <row r="6" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="48" t="s">
         <v>52</v>
       </c>
-      <c r="C6" s="57" t="s">
+      <c r="C6" s="58" t="s">
         <v>53</v>
       </c>
-      <c r="D6" s="58"/>
-      <c r="E6" s="58"/>
-      <c r="F6" s="59"/>
+      <c r="D6" s="59"/>
+      <c r="E6" s="59"/>
+      <c r="F6" s="60"/>
     </row>
     <row r="7" spans="2:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="71" t="s">
+      <c r="B7" s="49" t="s">
         <v>67</v>
       </c>
-      <c r="C7" s="72" t="s">
+      <c r="C7" s="71" t="s">
         <v>68</v>
       </c>
-      <c r="D7" s="73"/>
-      <c r="E7" s="73"/>
-      <c r="F7" s="74"/>
+      <c r="D7" s="72"/>
+      <c r="E7" s="72"/>
+      <c r="F7" s="73"/>
+      <c r="G7" s="1" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="8" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="C8" s="60" t="s">
+      <c r="C8" s="61" t="s">
         <v>50</v>
       </c>
-      <c r="D8" s="61"/>
-      <c r="E8" s="61"/>
-      <c r="F8" s="62"/>
+      <c r="D8" s="62"/>
+      <c r="E8" s="62"/>
+      <c r="F8" s="63"/>
     </row>
     <row r="9" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B9"/>
@@ -2268,42 +2274,42 @@
       <c r="G19"/>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B20" s="70" t="s">
+      <c r="B20" s="74" t="s">
         <v>69</v>
       </c>
-      <c r="C20" s="70"/>
-      <c r="D20" s="70"/>
-      <c r="E20" s="70"/>
-      <c r="F20" s="70"/>
-      <c r="G20" s="70"/>
-      <c r="H20" s="70"/>
+      <c r="C20" s="74"/>
+      <c r="D20" s="74"/>
+      <c r="E20" s="74"/>
+      <c r="F20" s="74"/>
+      <c r="G20" s="74"/>
+      <c r="H20" s="74"/>
     </row>
     <row r="21" spans="2:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="70"/>
-      <c r="C21" s="70"/>
-      <c r="D21" s="70"/>
-      <c r="E21" s="70"/>
-      <c r="F21" s="70"/>
-      <c r="G21" s="70"/>
-      <c r="H21" s="70"/>
+      <c r="B21" s="74"/>
+      <c r="C21" s="74"/>
+      <c r="D21" s="74"/>
+      <c r="E21" s="74"/>
+      <c r="F21" s="74"/>
+      <c r="G21" s="74"/>
+      <c r="H21" s="74"/>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B22" s="70"/>
-      <c r="C22" s="70"/>
-      <c r="D22" s="70"/>
-      <c r="E22" s="70"/>
-      <c r="F22" s="70"/>
-      <c r="G22" s="70"/>
-      <c r="H22" s="70"/>
+      <c r="B22" s="74"/>
+      <c r="C22" s="74"/>
+      <c r="D22" s="74"/>
+      <c r="E22" s="74"/>
+      <c r="F22" s="74"/>
+      <c r="G22" s="74"/>
+      <c r="H22" s="74"/>
     </row>
     <row r="23" spans="2:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="70"/>
-      <c r="C23" s="70"/>
-      <c r="D23" s="70"/>
-      <c r="E23" s="70"/>
-      <c r="F23" s="70"/>
-      <c r="G23" s="70"/>
-      <c r="H23" s="70"/>
+      <c r="B23" s="74"/>
+      <c r="C23" s="74"/>
+      <c r="D23" s="74"/>
+      <c r="E23" s="74"/>
+      <c r="F23" s="74"/>
+      <c r="G23" s="74"/>
+      <c r="H23" s="74"/>
     </row>
     <row r="24" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24"/>
@@ -2352,10 +2358,10 @@
       <c r="E26" s="44" t="s">
         <v>60</v>
       </c>
-      <c r="F26" s="63" t="s">
+      <c r="F26" s="64" t="s">
         <v>4</v>
       </c>
-      <c r="G26" s="66" t="s">
+      <c r="G26" s="67" t="s">
         <v>5</v>
       </c>
       <c r="H26" s="8" t="s">
@@ -2378,8 +2384,8 @@
       <c r="E27" s="45" t="s">
         <v>60</v>
       </c>
-      <c r="F27" s="64"/>
-      <c r="G27" s="67"/>
+      <c r="F27" s="65"/>
+      <c r="G27" s="68"/>
       <c r="H27" s="9" t="s">
         <v>16</v>
       </c>
@@ -2394,8 +2400,8 @@
       </c>
       <c r="D28" s="25"/>
       <c r="E28" s="36"/>
-      <c r="F28" s="64"/>
-      <c r="G28" s="67"/>
+      <c r="F28" s="65"/>
+      <c r="G28" s="68"/>
       <c r="H28" s="10" t="s">
         <v>17</v>
       </c>
@@ -2410,8 +2416,8 @@
       <c r="C29" s="25"/>
       <c r="D29" s="25"/>
       <c r="E29" s="36"/>
-      <c r="F29" s="64"/>
-      <c r="G29" s="67"/>
+      <c r="F29" s="65"/>
+      <c r="G29" s="68"/>
       <c r="H29" s="10" t="s">
         <v>18</v>
       </c>
@@ -2426,8 +2432,8 @@
         <v>60</v>
       </c>
       <c r="E30" s="36"/>
-      <c r="F30" s="64"/>
-      <c r="G30" s="67"/>
+      <c r="F30" s="65"/>
+      <c r="G30" s="68"/>
       <c r="H30" s="10" t="s">
         <v>19</v>
       </c>
@@ -2442,8 +2448,8 @@
       </c>
       <c r="D31" s="25"/>
       <c r="E31" s="36"/>
-      <c r="F31" s="64"/>
-      <c r="G31" s="67"/>
+      <c r="F31" s="65"/>
+      <c r="G31" s="68"/>
       <c r="H31" s="11" t="s">
         <v>20</v>
       </c>
@@ -2458,8 +2464,8 @@
       <c r="C32" s="25"/>
       <c r="D32" s="25"/>
       <c r="E32" s="36"/>
-      <c r="F32" s="64"/>
-      <c r="G32" s="67"/>
+      <c r="F32" s="65"/>
+      <c r="G32" s="68"/>
       <c r="H32" s="11" t="s">
         <v>21</v>
       </c>
@@ -2474,8 +2480,8 @@
         <v>60</v>
       </c>
       <c r="E33" s="36"/>
-      <c r="F33" s="64"/>
-      <c r="G33" s="67"/>
+      <c r="F33" s="65"/>
+      <c r="G33" s="68"/>
       <c r="H33" s="11" t="s">
         <v>22</v>
       </c>
@@ -2490,8 +2496,8 @@
       </c>
       <c r="D34" s="25"/>
       <c r="E34" s="36"/>
-      <c r="F34" s="64"/>
-      <c r="G34" s="67"/>
+      <c r="F34" s="65"/>
+      <c r="G34" s="68"/>
       <c r="H34" s="12" t="s">
         <v>23</v>
       </c>
@@ -2506,8 +2512,8 @@
       <c r="C35" s="25"/>
       <c r="D35" s="25"/>
       <c r="E35" s="36"/>
-      <c r="F35" s="64"/>
-      <c r="G35" s="67"/>
+      <c r="F35" s="65"/>
+      <c r="G35" s="68"/>
       <c r="H35" s="12" t="s">
         <v>24</v>
       </c>
@@ -2522,8 +2528,8 @@
         <v>60</v>
       </c>
       <c r="E36" s="36"/>
-      <c r="F36" s="64"/>
-      <c r="G36" s="67"/>
+      <c r="F36" s="65"/>
+      <c r="G36" s="68"/>
       <c r="H36" s="12" t="s">
         <v>25</v>
       </c>
@@ -2538,8 +2544,8 @@
       <c r="E37" s="45" t="s">
         <v>60</v>
       </c>
-      <c r="F37" s="64"/>
-      <c r="G37" s="67"/>
+      <c r="F37" s="65"/>
+      <c r="G37" s="68"/>
       <c r="H37" s="12" t="s">
         <v>61</v>
       </c>
@@ -2560,8 +2566,8 @@
       <c r="E38" s="45" t="s">
         <v>60</v>
       </c>
-      <c r="F38" s="64"/>
-      <c r="G38" s="67"/>
+      <c r="F38" s="65"/>
+      <c r="G38" s="68"/>
       <c r="H38" s="13" t="s">
         <v>26</v>
       </c>
@@ -2582,8 +2588,8 @@
       <c r="E39" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="F39" s="65"/>
-      <c r="G39" s="68"/>
+      <c r="F39" s="66"/>
+      <c r="G39" s="69"/>
       <c r="H39" s="14" t="s">
         <v>27</v>
       </c>
@@ -2598,10 +2604,10 @@
       </c>
       <c r="D40" s="33"/>
       <c r="E40" s="34"/>
-      <c r="F40" s="63" t="s">
+      <c r="F40" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="G40" s="66" t="s">
+      <c r="G40" s="67" t="s">
         <v>7</v>
       </c>
       <c r="H40" s="15" t="s">
@@ -2618,8 +2624,8 @@
       <c r="C41" s="25"/>
       <c r="D41" s="25"/>
       <c r="E41" s="36"/>
-      <c r="F41" s="69"/>
-      <c r="G41" s="67"/>
+      <c r="F41" s="70"/>
+      <c r="G41" s="68"/>
       <c r="H41" s="16" t="s">
         <v>36</v>
       </c>
@@ -2634,8 +2640,8 @@
         <v>60</v>
       </c>
       <c r="E42" s="40"/>
-      <c r="F42" s="65"/>
-      <c r="G42" s="68"/>
+      <c r="F42" s="66"/>
+      <c r="G42" s="69"/>
       <c r="H42" s="17" t="s">
         <v>37</v>
       </c>
@@ -2650,10 +2656,10 @@
       <c r="C43" s="33"/>
       <c r="D43" s="33"/>
       <c r="E43" s="34"/>
-      <c r="F43" s="63" t="s">
+      <c r="F43" s="64" t="s">
         <v>8</v>
       </c>
-      <c r="G43" s="66" t="s">
+      <c r="G43" s="67" t="s">
         <v>9</v>
       </c>
       <c r="H43" s="18" t="s">
@@ -2670,8 +2676,8 @@
       </c>
       <c r="D44" s="25"/>
       <c r="E44" s="36"/>
-      <c r="F44" s="69"/>
-      <c r="G44" s="67"/>
+      <c r="F44" s="70"/>
+      <c r="G44" s="68"/>
       <c r="H44" s="19" t="s">
         <v>39</v>
       </c>
@@ -2686,8 +2692,8 @@
         <v>60</v>
       </c>
       <c r="E45" s="40"/>
-      <c r="F45" s="65"/>
-      <c r="G45" s="68"/>
+      <c r="F45" s="66"/>
+      <c r="G45" s="69"/>
       <c r="H45" s="20" t="s">
         <v>40</v>
       </c>
@@ -2706,10 +2712,10 @@
         <v>60</v>
       </c>
       <c r="E46" s="28"/>
-      <c r="F46" s="50" t="s">
+      <c r="F46" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="G46" s="52" t="s">
+      <c r="G46" s="53" t="s">
         <v>10</v>
       </c>
       <c r="H46" s="21" t="s">
@@ -2726,8 +2732,8 @@
       <c r="E47" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="F47" s="51"/>
-      <c r="G47" s="53"/>
+      <c r="F47" s="52"/>
+      <c r="G47" s="54"/>
       <c r="H47" s="22" t="s">
         <v>73</v>
       </c>
@@ -2736,6 +2742,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A25:I47"/>
   <mergeCells count="15">
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="F46:F47"/>

</xml_diff>

<commit_message>
Updated notes and technical req doc
</commit_message>
<xml_diff>
--- a/data_architect_misc/kf_generator/Key-Figures_Files_Req_Specification.xlsx
+++ b/data_architect_misc/kf_generator/Key-Figures_Files_Req_Specification.xlsx
@@ -1025,7 +1025,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1110,6 +1110,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="34">
     <border>
@@ -1554,15 +1560,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1764,6 +1761,15 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1803,7 +1809,7 @@
         <xdr:cNvPr id="2" name="Imagen 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{921CB379-B0A3-4CB7-AAE9-974F0EDBB619}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{921CB379-B0A3-4CB7-AAE9-974F0EDBB619}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2102,8 +2108,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C44" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G46" sqref="G46:G47"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I47" sqref="I47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="88.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2120,74 +2126,74 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="23.25" x14ac:dyDescent="0.2">
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="47" t="s">
         <v>62</v>
       </c>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
     </row>
     <row r="3" spans="2:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="48" t="s">
+      <c r="B4" s="45" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="55" t="s">
+      <c r="C4" s="52" t="s">
         <v>63</v>
       </c>
-      <c r="D4" s="56"/>
-      <c r="E4" s="56"/>
-      <c r="F4" s="57"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="54"/>
     </row>
     <row r="5" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="48" t="s">
+      <c r="B5" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="C5" s="58" t="s">
+      <c r="C5" s="55" t="s">
         <v>48</v>
       </c>
-      <c r="D5" s="59"/>
-      <c r="E5" s="59"/>
-      <c r="F5" s="60"/>
+      <c r="D5" s="56"/>
+      <c r="E5" s="56"/>
+      <c r="F5" s="57"/>
     </row>
     <row r="6" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="48" t="s">
+      <c r="B6" s="45" t="s">
         <v>52</v>
       </c>
-      <c r="C6" s="58" t="s">
+      <c r="C6" s="55" t="s">
         <v>53</v>
       </c>
-      <c r="D6" s="59"/>
-      <c r="E6" s="59"/>
-      <c r="F6" s="60"/>
+      <c r="D6" s="56"/>
+      <c r="E6" s="56"/>
+      <c r="F6" s="57"/>
     </row>
     <row r="7" spans="2:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="49" t="s">
+      <c r="B7" s="46" t="s">
         <v>67</v>
       </c>
-      <c r="C7" s="71" t="s">
+      <c r="C7" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="D7" s="72"/>
-      <c r="E7" s="72"/>
-      <c r="F7" s="73"/>
+      <c r="D7" s="69"/>
+      <c r="E7" s="69"/>
+      <c r="F7" s="70"/>
       <c r="G7" s="1" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="8" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="48" t="s">
+      <c r="B8" s="45" t="s">
         <v>49</v>
       </c>
-      <c r="C8" s="61" t="s">
+      <c r="C8" s="58" t="s">
         <v>50</v>
       </c>
-      <c r="D8" s="62"/>
-      <c r="E8" s="62"/>
-      <c r="F8" s="63"/>
+      <c r="D8" s="59"/>
+      <c r="E8" s="59"/>
+      <c r="F8" s="60"/>
     </row>
     <row r="9" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B9"/>
@@ -2202,7 +2208,7 @@
       <c r="E10"/>
     </row>
     <row r="11" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="20" t="s">
         <v>55</v>
       </c>
       <c r="C11"/>
@@ -2274,42 +2280,42 @@
       <c r="G19"/>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B20" s="74" t="s">
+      <c r="B20" s="71" t="s">
         <v>69</v>
       </c>
-      <c r="C20" s="74"/>
-      <c r="D20" s="74"/>
-      <c r="E20" s="74"/>
-      <c r="F20" s="74"/>
-      <c r="G20" s="74"/>
-      <c r="H20" s="74"/>
+      <c r="C20" s="71"/>
+      <c r="D20" s="71"/>
+      <c r="E20" s="71"/>
+      <c r="F20" s="71"/>
+      <c r="G20" s="71"/>
+      <c r="H20" s="71"/>
     </row>
     <row r="21" spans="2:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="74"/>
-      <c r="C21" s="74"/>
-      <c r="D21" s="74"/>
-      <c r="E21" s="74"/>
-      <c r="F21" s="74"/>
-      <c r="G21" s="74"/>
-      <c r="H21" s="74"/>
+      <c r="B21" s="71"/>
+      <c r="C21" s="71"/>
+      <c r="D21" s="71"/>
+      <c r="E21" s="71"/>
+      <c r="F21" s="71"/>
+      <c r="G21" s="71"/>
+      <c r="H21" s="71"/>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B22" s="74"/>
-      <c r="C22" s="74"/>
-      <c r="D22" s="74"/>
-      <c r="E22" s="74"/>
-      <c r="F22" s="74"/>
-      <c r="G22" s="74"/>
-      <c r="H22" s="74"/>
+      <c r="B22" s="71"/>
+      <c r="C22" s="71"/>
+      <c r="D22" s="71"/>
+      <c r="E22" s="71"/>
+      <c r="F22" s="71"/>
+      <c r="G22" s="71"/>
+      <c r="H22" s="71"/>
     </row>
     <row r="23" spans="2:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="74"/>
-      <c r="C23" s="74"/>
-      <c r="D23" s="74"/>
-      <c r="E23" s="74"/>
-      <c r="F23" s="74"/>
-      <c r="G23" s="74"/>
-      <c r="H23" s="74"/>
+      <c r="B23" s="71"/>
+      <c r="C23" s="71"/>
+      <c r="D23" s="71"/>
+      <c r="E23" s="71"/>
+      <c r="F23" s="71"/>
+      <c r="G23" s="71"/>
+      <c r="H23" s="71"/>
     </row>
     <row r="24" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24"/>
@@ -2346,398 +2352,398 @@
       </c>
     </row>
     <row r="26" spans="2:9" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="B26" s="32" t="s">
-        <v>60</v>
-      </c>
-      <c r="C26" s="42" t="s">
-        <v>60</v>
-      </c>
-      <c r="D26" s="42" t="s">
-        <v>60</v>
-      </c>
-      <c r="E26" s="44" t="s">
-        <v>60</v>
-      </c>
-      <c r="F26" s="64" t="s">
+      <c r="B26" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="C26" s="39" t="s">
+        <v>60</v>
+      </c>
+      <c r="D26" s="39" t="s">
+        <v>60</v>
+      </c>
+      <c r="E26" s="41" t="s">
+        <v>60</v>
+      </c>
+      <c r="F26" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="G26" s="67" t="s">
+      <c r="G26" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="H26" s="8" t="s">
+      <c r="H26" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I26" s="3" t="s">
+      <c r="I26" s="73" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="27" spans="2:9" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="B27" s="43" t="s">
-        <v>60</v>
-      </c>
-      <c r="C27" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="D27" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="E27" s="45" t="s">
-        <v>60</v>
-      </c>
-      <c r="F27" s="65"/>
-      <c r="G27" s="68"/>
-      <c r="H27" s="9" t="s">
+      <c r="B27" s="40" t="s">
+        <v>60</v>
+      </c>
+      <c r="C27" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D27" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="E27" s="42" t="s">
+        <v>60</v>
+      </c>
+      <c r="F27" s="62"/>
+      <c r="G27" s="65"/>
+      <c r="H27" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I27" s="4" t="s">
+      <c r="I27" s="72" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="28" spans="2:9" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="B28" s="35"/>
-      <c r="C28" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="D28" s="25"/>
-      <c r="E28" s="36"/>
-      <c r="F28" s="65"/>
-      <c r="G28" s="68"/>
-      <c r="H28" s="10" t="s">
+      <c r="B28" s="32"/>
+      <c r="C28" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D28" s="22"/>
+      <c r="E28" s="33"/>
+      <c r="F28" s="62"/>
+      <c r="G28" s="65"/>
+      <c r="H28" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="I28" s="4" t="s">
+      <c r="I28" s="72" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="29" spans="2:9" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="B29" s="43" t="s">
-        <v>60</v>
-      </c>
-      <c r="C29" s="25"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="36"/>
-      <c r="F29" s="65"/>
-      <c r="G29" s="68"/>
-      <c r="H29" s="10" t="s">
+      <c r="B29" s="40" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29" s="22"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="33"/>
+      <c r="F29" s="62"/>
+      <c r="G29" s="65"/>
+      <c r="H29" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="I29" s="4" t="s">
+      <c r="I29" s="72" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="30" spans="2:9" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="B30" s="35"/>
-      <c r="C30" s="25"/>
-      <c r="D30" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="E30" s="36"/>
-      <c r="F30" s="65"/>
-      <c r="G30" s="68"/>
-      <c r="H30" s="10" t="s">
+      <c r="B30" s="32"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="E30" s="33"/>
+      <c r="F30" s="62"/>
+      <c r="G30" s="65"/>
+      <c r="H30" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="I30" s="4" t="s">
+      <c r="I30" s="72" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="31" spans="2:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B31" s="35"/>
-      <c r="C31" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="D31" s="25"/>
-      <c r="E31" s="36"/>
-      <c r="F31" s="65"/>
-      <c r="G31" s="68"/>
-      <c r="H31" s="11" t="s">
+      <c r="B31" s="32"/>
+      <c r="C31" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D31" s="22"/>
+      <c r="E31" s="33"/>
+      <c r="F31" s="62"/>
+      <c r="G31" s="65"/>
+      <c r="H31" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="I31" s="4" t="s">
+      <c r="I31" s="72" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="32" spans="2:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B32" s="43" t="s">
-        <v>60</v>
-      </c>
-      <c r="C32" s="25"/>
-      <c r="D32" s="25"/>
-      <c r="E32" s="36"/>
-      <c r="F32" s="65"/>
-      <c r="G32" s="68"/>
-      <c r="H32" s="11" t="s">
+      <c r="B32" s="40" t="s">
+        <v>60</v>
+      </c>
+      <c r="C32" s="22"/>
+      <c r="D32" s="22"/>
+      <c r="E32" s="33"/>
+      <c r="F32" s="62"/>
+      <c r="G32" s="65"/>
+      <c r="H32" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="I32" s="4" t="s">
+      <c r="I32" s="72" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="33" spans="2:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B33" s="35"/>
-      <c r="C33" s="25"/>
-      <c r="D33" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="E33" s="36"/>
-      <c r="F33" s="65"/>
-      <c r="G33" s="68"/>
-      <c r="H33" s="11" t="s">
+      <c r="B33" s="32"/>
+      <c r="C33" s="22"/>
+      <c r="D33" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="E33" s="33"/>
+      <c r="F33" s="62"/>
+      <c r="G33" s="65"/>
+      <c r="H33" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="I33" s="4" t="s">
+      <c r="I33" s="72" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="34" spans="2:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B34" s="35"/>
-      <c r="C34" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="D34" s="25"/>
-      <c r="E34" s="36"/>
-      <c r="F34" s="65"/>
-      <c r="G34" s="68"/>
-      <c r="H34" s="12" t="s">
+      <c r="B34" s="32"/>
+      <c r="C34" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D34" s="22"/>
+      <c r="E34" s="33"/>
+      <c r="F34" s="62"/>
+      <c r="G34" s="65"/>
+      <c r="H34" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="I34" s="4" t="s">
+      <c r="I34" s="72" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="35" spans="2:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B35" s="43" t="s">
-        <v>60</v>
-      </c>
-      <c r="C35" s="25"/>
-      <c r="D35" s="25"/>
-      <c r="E35" s="36"/>
-      <c r="F35" s="65"/>
-      <c r="G35" s="68"/>
-      <c r="H35" s="12" t="s">
+      <c r="B35" s="40" t="s">
+        <v>60</v>
+      </c>
+      <c r="C35" s="22"/>
+      <c r="D35" s="22"/>
+      <c r="E35" s="33"/>
+      <c r="F35" s="62"/>
+      <c r="G35" s="65"/>
+      <c r="H35" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="I35" s="4" t="s">
+      <c r="I35" s="72" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="36" spans="2:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B36" s="35"/>
-      <c r="C36" s="25"/>
-      <c r="D36" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="E36" s="36"/>
-      <c r="F36" s="65"/>
-      <c r="G36" s="68"/>
-      <c r="H36" s="12" t="s">
+      <c r="B36" s="32"/>
+      <c r="C36" s="22"/>
+      <c r="D36" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="E36" s="33"/>
+      <c r="F36" s="62"/>
+      <c r="G36" s="65"/>
+      <c r="H36" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="I36" s="4" t="s">
+      <c r="I36" s="72" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B37" s="35"/>
-      <c r="C37" s="25"/>
-      <c r="D37" s="25"/>
-      <c r="E37" s="45" t="s">
-        <v>60</v>
-      </c>
-      <c r="F37" s="65"/>
-      <c r="G37" s="68"/>
-      <c r="H37" s="12" t="s">
+      <c r="B37" s="32"/>
+      <c r="C37" s="22"/>
+      <c r="D37" s="22"/>
+      <c r="E37" s="42" t="s">
+        <v>60</v>
+      </c>
+      <c r="F37" s="62"/>
+      <c r="G37" s="65"/>
+      <c r="H37" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="I37" s="4" t="s">
+      <c r="I37" s="72" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B38" s="43" t="s">
-        <v>60</v>
-      </c>
-      <c r="C38" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="D38" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="E38" s="45" t="s">
-        <v>60</v>
-      </c>
-      <c r="F38" s="65"/>
-      <c r="G38" s="68"/>
-      <c r="H38" s="13" t="s">
+      <c r="B38" s="40" t="s">
+        <v>60</v>
+      </c>
+      <c r="C38" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D38" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="E38" s="42" t="s">
+        <v>60</v>
+      </c>
+      <c r="F38" s="62"/>
+      <c r="G38" s="65"/>
+      <c r="H38" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="I38" s="4" t="s">
+      <c r="I38" s="72" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="39" spans="2:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="46" t="s">
-        <v>60</v>
-      </c>
-      <c r="C39" s="39" t="s">
-        <v>60</v>
-      </c>
-      <c r="D39" s="39" t="s">
-        <v>60</v>
-      </c>
-      <c r="E39" s="47" t="s">
-        <v>60</v>
-      </c>
-      <c r="F39" s="66"/>
-      <c r="G39" s="69"/>
-      <c r="H39" s="14" t="s">
+      <c r="B39" s="43" t="s">
+        <v>60</v>
+      </c>
+      <c r="C39" s="36" t="s">
+        <v>60</v>
+      </c>
+      <c r="D39" s="36" t="s">
+        <v>60</v>
+      </c>
+      <c r="E39" s="44" t="s">
+        <v>60</v>
+      </c>
+      <c r="F39" s="63"/>
+      <c r="G39" s="66"/>
+      <c r="H39" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="I39" s="5" t="s">
+      <c r="I39" s="74" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="40" spans="2:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B40" s="41"/>
-      <c r="C40" s="42" t="s">
-        <v>60</v>
-      </c>
-      <c r="D40" s="33"/>
-      <c r="E40" s="34"/>
-      <c r="F40" s="64" t="s">
+      <c r="B40" s="38"/>
+      <c r="C40" s="39" t="s">
+        <v>60</v>
+      </c>
+      <c r="D40" s="30"/>
+      <c r="E40" s="31"/>
+      <c r="F40" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="G40" s="67" t="s">
+      <c r="G40" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="H40" s="15" t="s">
+      <c r="H40" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="I40" s="3" t="s">
+      <c r="I40" s="73" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="41" spans="2:9" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="B41" s="43" t="s">
-        <v>60</v>
-      </c>
-      <c r="C41" s="25"/>
-      <c r="D41" s="25"/>
-      <c r="E41" s="36"/>
-      <c r="F41" s="70"/>
-      <c r="G41" s="68"/>
-      <c r="H41" s="16" t="s">
+      <c r="B41" s="40" t="s">
+        <v>60</v>
+      </c>
+      <c r="C41" s="22"/>
+      <c r="D41" s="22"/>
+      <c r="E41" s="33"/>
+      <c r="F41" s="67"/>
+      <c r="G41" s="65"/>
+      <c r="H41" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="I41" s="4" t="s">
+      <c r="I41" s="72" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="42" spans="2:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="37"/>
-      <c r="C42" s="38"/>
-      <c r="D42" s="39" t="s">
-        <v>60</v>
-      </c>
-      <c r="E42" s="40"/>
-      <c r="F42" s="66"/>
-      <c r="G42" s="69"/>
-      <c r="H42" s="17" t="s">
+      <c r="B42" s="34"/>
+      <c r="C42" s="35"/>
+      <c r="D42" s="36" t="s">
+        <v>60</v>
+      </c>
+      <c r="E42" s="37"/>
+      <c r="F42" s="63"/>
+      <c r="G42" s="66"/>
+      <c r="H42" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="I42" s="5" t="s">
+      <c r="I42" s="74" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="43" spans="2:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B43" s="32" t="s">
-        <v>60</v>
-      </c>
-      <c r="C43" s="33"/>
-      <c r="D43" s="33"/>
-      <c r="E43" s="34"/>
-      <c r="F43" s="64" t="s">
+      <c r="B43" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="C43" s="30"/>
+      <c r="D43" s="30"/>
+      <c r="E43" s="31"/>
+      <c r="F43" s="61" t="s">
         <v>8</v>
       </c>
-      <c r="G43" s="67" t="s">
+      <c r="G43" s="64" t="s">
         <v>9</v>
       </c>
-      <c r="H43" s="18" t="s">
+      <c r="H43" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="I43" s="3" t="s">
+      <c r="I43" s="73" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="44" spans="2:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B44" s="35"/>
-      <c r="C44" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="D44" s="25"/>
-      <c r="E44" s="36"/>
-      <c r="F44" s="70"/>
-      <c r="G44" s="68"/>
-      <c r="H44" s="19" t="s">
+      <c r="B44" s="32"/>
+      <c r="C44" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D44" s="22"/>
+      <c r="E44" s="33"/>
+      <c r="F44" s="67"/>
+      <c r="G44" s="65"/>
+      <c r="H44" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="I44" s="4" t="s">
+      <c r="I44" s="72" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="45" spans="2:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="37"/>
-      <c r="C45" s="38"/>
-      <c r="D45" s="39" t="s">
-        <v>60</v>
-      </c>
-      <c r="E45" s="40"/>
-      <c r="F45" s="66"/>
-      <c r="G45" s="69"/>
-      <c r="H45" s="20" t="s">
+      <c r="B45" s="34"/>
+      <c r="C45" s="35"/>
+      <c r="D45" s="36" t="s">
+        <v>60</v>
+      </c>
+      <c r="E45" s="37"/>
+      <c r="F45" s="63"/>
+      <c r="G45" s="66"/>
+      <c r="H45" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="I45" s="5" t="s">
+      <c r="I45" s="74" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="46" spans="2:9" ht="244.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="26" t="s">
-        <v>60</v>
-      </c>
-      <c r="C46" s="27" t="s">
-        <v>60</v>
-      </c>
-      <c r="D46" s="27" t="s">
-        <v>60</v>
-      </c>
-      <c r="E46" s="28"/>
-      <c r="F46" s="51" t="s">
+      <c r="B46" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="C46" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="D46" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="E46" s="25"/>
+      <c r="F46" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="G46" s="53" t="s">
+      <c r="G46" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="H46" s="21" t="s">
+      <c r="H46" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="I46" s="6" t="s">
+      <c r="I46" s="3" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="47" spans="2:9" ht="244.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="29"/>
-      <c r="C47" s="30"/>
-      <c r="D47" s="30"/>
-      <c r="E47" s="31" t="s">
-        <v>60</v>
-      </c>
-      <c r="F47" s="52"/>
-      <c r="G47" s="54"/>
-      <c r="H47" s="22" t="s">
+      <c r="B47" s="26"/>
+      <c r="C47" s="27"/>
+      <c r="D47" s="27"/>
+      <c r="E47" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="F47" s="49"/>
+      <c r="G47" s="51"/>
+      <c r="H47" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="I47" s="7" t="s">
+      <c r="I47" s="4" t="s">
         <v>64</v>
       </c>
     </row>

</xml_diff>